<commit_message>
fix bug contract baru
</commit_message>
<xml_diff>
--- a/public/EmployeeData/template-employee-fix-banget.xlsx
+++ b/public/EmployeeData/template-employee-fix-banget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49082036-54CE-6248-B45B-B921724408AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4B425E-5C08-B14E-9928-637446549CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -95,12 +95,6 @@
     <t>kr9@contoh.com</t>
   </si>
   <si>
-    <t>graha-segara-belawan</t>
-  </si>
-  <si>
-    <t>graha-segara</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
@@ -143,16 +137,10 @@
     <t>Gol Darah</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Kontrak</t>
-  </si>
-  <si>
-    <t>Tetap</t>
-  </si>
-  <si>
     <t>Islam</t>
+  </si>
+  <si>
+    <t>Graha-Segara-Belawan</t>
   </si>
 </sst>
 </file>
@@ -668,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="134" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="134" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -686,14 +674,14 @@
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.1640625" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,40 +719,37 @@
         <v>14</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -787,26 +772,24 @@
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="M2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -815,9 +798,8 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -840,26 +822,24 @@
         <v>9</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="L3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>39</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -868,9 +848,8 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -879,7 +858,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -888,7 +867,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -898,7 +877,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -907,7 +886,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -916,7 +895,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>

</xml_diff>